<commit_message>
update RF and GBM v3 and modify results in poster
</commit_message>
<xml_diff>
--- a/data/model performance.xlsx
+++ b/data/model performance.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\miran\Downloads\dsan5550-final-project\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3373397-A270-4158-B9EE-044835DCE6FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{602FAB4E-2504-4FA8-B0A0-A5931B1C3E51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30612" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -75,10 +75,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="178" formatCode="0.000_ "/>
+  <numFmts count="2">
+    <numFmt numFmtId="176" formatCode="0.000_ "/>
+    <numFmt numFmtId="177" formatCode="0.000_);[Red]\(0.000\)"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -91,6 +92,13 @@
       <name val="等线"/>
       <family val="3"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="等线"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -114,23 +122,31 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="5">
     <dxf>
+      <numFmt numFmtId="177" formatCode="0.000_);[Red]\(0.000\)"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="176" formatCode="0.000_ "/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -433,14 +449,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" zoomScale="158" zoomScaleNormal="158" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="30.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.77734375" customWidth="1"/>
+    <col min="3" max="3" width="8.88671875" style="3"/>
+    <col min="4" max="4" width="11.77734375" style="4" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -450,10 +467,10 @@
       <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="6" t="s">
         <v>2</v>
       </c>
     </row>
@@ -464,10 +481,10 @@
       <c r="B2" s="1">
         <v>0.74199999999999999</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="2">
         <v>0.57699999999999996</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D2" s="5">
         <v>0.754</v>
       </c>
     </row>
@@ -478,10 +495,10 @@
       <c r="B3" s="1">
         <v>0.51400000000000001</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3" s="2">
         <v>0.41599999999999998</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D3" s="5">
         <v>0.88200000000000001</v>
       </c>
     </row>
@@ -490,13 +507,13 @@
         <v>5</v>
       </c>
       <c r="B4" s="1">
-        <v>0.112</v>
-      </c>
-      <c r="C4" s="1">
-        <v>8.7999999999999995E-2</v>
-      </c>
-      <c r="D4" s="1">
-        <v>0.99399999999999999</v>
+        <v>0.155</v>
+      </c>
+      <c r="C4" s="2">
+        <v>0.129</v>
+      </c>
+      <c r="D4" s="5">
+        <v>0.98899999999999999</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -504,13 +521,13 @@
         <v>6</v>
       </c>
       <c r="B5" s="1">
-        <v>0.11799999999999999</v>
-      </c>
-      <c r="C5" s="1">
-        <v>9.5000000000000001E-2</v>
-      </c>
-      <c r="D5" s="1">
-        <v>0.99399999999999999</v>
+        <v>0.21099999999999999</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0.18</v>
+      </c>
+      <c r="D5" s="5">
+        <v>0.98</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -520,10 +537,10 @@
       <c r="B6" s="1">
         <v>0.69099999999999995</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6" s="2">
         <v>0.58699999999999997</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D6" s="5">
         <v>0.78600000000000003</v>
       </c>
     </row>
@@ -534,10 +551,10 @@
       <c r="B7" s="1">
         <v>0.58399999999999996</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7" s="2">
         <v>0.495</v>
       </c>
-      <c r="D7" s="1">
+      <c r="D7" s="5">
         <v>0.84699999999999998</v>
       </c>
     </row>
@@ -548,10 +565,10 @@
       <c r="B8" s="1">
         <v>0.33800000000000002</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8" s="2">
         <v>0.24099999999999999</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D8" s="5">
         <v>0.95</v>
       </c>
     </row>

</xml_diff>

<commit_message>
deploy SARIMA RF GBM prediction to other stations
</commit_message>
<xml_diff>
--- a/data/model performance.xlsx
+++ b/data/model performance.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\miran\Downloads\dsan5550-final-project\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{602FAB4E-2504-4FA8-B0A0-A5931B1C3E51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDFB3946-05A0-45A0-B64D-2C4E7B5B9002}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30612" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12372" yWindow="3516" windowWidth="15360" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -450,7 +450,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="158" zoomScaleNormal="158" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>

</xml_diff>